<commit_message>
Acrescentado content negotiation com XML e YAML, Dado inicio a implementação de HATEOAS
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -685,7 +685,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -743,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -754,7 +754,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -765,7 +765,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Começando a adicionar a documentação da API com o OpenAPI Swagger
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -204,7 +204,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -684,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +795,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -776,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -960,68 +990,68 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="C29:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C17">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C28">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finalizado a implementação do Swagger da OpenAPI e iniciado os testes de integração
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxuel\Desktop\rest-pdv-padaria\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A598697-536B-4E57-A346-A47009E7ADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="4710" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -48,9 +54,6 @@
     <t>Implementar HATEOAS</t>
   </si>
   <si>
-    <t>Implementar Swagger OpenAPI</t>
-  </si>
-  <si>
     <t>Configurar CORS</t>
   </si>
   <si>
@@ -76,12 +79,15 @@
   </si>
   <si>
     <t>Emissão de Cupom fiscal</t>
+  </si>
+  <si>
+    <t>Implementar Swagger OpenAPI e testes de integração</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,37 +210,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -420,6 +396,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -428,7 +407,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -466,9 +445,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,9 +480,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,9 +532,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -711,11 +724,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,12 +811,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
@@ -814,7 +827,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -825,7 +838,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -836,7 +849,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -847,7 +860,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
@@ -858,7 +871,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -869,7 +882,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -880,7 +893,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
@@ -891,7 +904,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
@@ -902,7 +915,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
@@ -990,68 +1003,68 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="C29:C1048576">
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C17">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C28">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1061,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1073,7 +1086,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Implementação do accessToken e quase finalizado o refreshToken
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxuel\Desktop\rest-pdv-padaria\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A598697-536B-4E57-A346-A47009E7ADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4710" yWindow="4215" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -87,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,7 +401,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -445,9 +439,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -480,26 +474,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,26 +509,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -724,11 +684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +779,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -830,7 +790,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -841,7 +801,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1074,7 +1034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1086,7 +1046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Resolvendo problema de Forbidden, que no caso era apenas um erro de digitação na classe AuthController, alterado todas os controllers alterandoo caminho de Request para /api/nome_da_request e resolvido problema de login onde não estava funcionando as senhas geradas pelo pbkdf2Encoder
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -688,7 +688,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +801,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -812,7 +812,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adicionado regra de permissão para acessar as paginas de acordo com a permissão do usuario
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -688,7 +688,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +812,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -823,7 +823,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Continuação dos testes de integração dos controllers
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -204,7 +204,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -688,7 +718,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +864,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -963,68 +993,68 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="C29:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C17">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C28">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finalizado o teste de integração dos controllers com JSON, XML e YML
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxuel\Desktop\rest-pdv-padaria\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC86356-1621-43B6-A26C-B2298707B33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="4215" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -81,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,37 +210,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -431,7 +407,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -469,9 +445,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,9 +480,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,9 +532,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -714,11 +724,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +863,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -993,68 +1003,68 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="C29:C1048576">
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C17">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C28">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Não realizado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1064,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1076,7 +1086,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Finalizado em partes o back end, e dado inicio ao front com React
</commit_message>
<xml_diff>
--- a/check list back-end.xlsx
+++ b/check list back-end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxuel\Desktop\rest-pdv-padaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC86356-1621-43B6-A26C-B2298707B33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC948891-07CB-4D4A-BBE9-ED272C7B9F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,7 +728,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +874,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -885,7 +885,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -896,7 +896,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -907,7 +907,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>